<commit_message>
Update test case #308
</commit_message>
<xml_diff>
--- a/Document/Reports/Report 5/Test case- TriPQM.xlsx
+++ b/Document/Reports/Report 5/Test case- TriPQM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -55,27 +55,6 @@
     <t>RNC3</t>
   </si>
   <si>
-    <t>1. Input valid information
-2. Create new contract</t>
-  </si>
-  <si>
-    <t>1. Input new contract information with an exist plate number
-2. Create new contract</t>
-  </si>
-  <si>
-    <t>Create contract successful, send an email contains customer code and password to customer. Show payment page.</t>
-  </si>
-  <si>
-    <t>Create contract unsuccessful. Show exist plate number error.</t>
-  </si>
-  <si>
-    <t>1. Input new contract information with an exist email
-2. Create new contract</t>
-  </si>
-  <si>
-    <t>Create contract unsuccessful. Show exist email error.</t>
-  </si>
-  <si>
     <t>1.2. &lt;Guest&gt; Register new contract payment</t>
   </si>
   <si>
@@ -88,27 +67,7 @@
     <t>RNCP2</t>
   </si>
   <si>
-    <t>Create Payment record, update contract status. Show success message.</t>
-  </si>
-  <si>
     <t>RNCP3</t>
-  </si>
-  <si>
-    <t>Show message to notify that guest has canceled the transaction.</t>
-  </si>
-  <si>
-    <t>1. Guest registered contract succeed.
-2. Guest choose direct payment.</t>
-  </si>
-  <si>
-    <t>1. Guest registered contract succeed.
-2. Guest choose PayPal payment.
-3. PayPal payment successful.</t>
-  </si>
-  <si>
-    <t>1. Guest registered contract succeed.
-2. Guest choose PayPal payment.
-3. Guest cancel transaction</t>
   </si>
   <si>
     <t>2.8. &lt;Staff&gt; View new card requests</t>
@@ -141,13 +100,7 @@
     <t>Test list new card request in ascending order of request date.</t>
   </si>
   <si>
-    <t>Display the list in ascending order of request date.</t>
-  </si>
-  <si>
     <t>Test unresolved request will be on top.</t>
-  </si>
-  <si>
-    <t>Display 3 unresolved request on top.</t>
   </si>
   <si>
     <t>2.9. &lt;Staff&gt; Resolve new card request</t>
@@ -159,61 +112,16 @@
     <t>SNCR1</t>
   </si>
   <si>
-    <t>1. Create 5 new card request with 5 different request date.
-2. View new card requests</t>
-  </si>
-  <si>
-    <t>1. Crete 5 new card request with the same request date. But 2 of them is resolved.
-2. View new card requests.</t>
-  </si>
-  <si>
-    <t>Create new card request record and the old card been deactivated.</t>
-  </si>
-  <si>
-    <t>Test send new card and deactivate old card request.</t>
-  </si>
-  <si>
     <t>SNCR2</t>
-  </si>
-  <si>
-    <t>Test send new card request.</t>
-  </si>
-  <si>
-    <t>1. Contract HD0001 having an actived card. No new card request before.
-2. Send new card request and deactivate old card request for contract HD0001.</t>
-  </si>
-  <si>
-    <t>1. Contract HD0001 having an actived card. No new card request before.
-2. Send new card request for contract HD0001.</t>
-  </si>
-  <si>
-    <t>Create new card request record</t>
   </si>
   <si>
     <t>SNCR3</t>
   </si>
   <si>
-    <t>1. Contract HD0001 having an actived card. No new card request before.
-2. Send new card request and delivery request.</t>
-  </si>
-  <si>
-    <t>Create new card request record with column "is_delivery_requested" = 1.</t>
-  </si>
-  <si>
     <t>SNCR4</t>
   </si>
   <si>
-    <t>Test send new card and delivery request.</t>
-  </si>
-  <si>
     <t>Test send new card request for a card already had another new card request before.</t>
-  </si>
-  <si>
-    <t>1. Contract HD0001 having an actived card with a new card request before.
-2. Send new card request for contract HD0001.</t>
-  </si>
-  <si>
-    <t>Show error message to notify that the card already had a new card request before.</t>
   </si>
   <si>
     <t>SNCR5</t>
@@ -222,11 +130,253 @@
     <t>Test send new card request for a contract have no card.</t>
   </si>
   <si>
-    <t>1. Contract HD0001 not having a card.
-2. Send new card request for contract HD0001.</t>
+    <t>1. Go to the home page
+2. Enter personal information:
+- Họ tên: Nguyễn Văn A
+- Email: baohiem@yahoo.com
+- Số điện thoại:0909099099
+- Số CMND/Hộ chiếu: 272185738
+- Địa chỉ: 123 Chợ Lớn, Bến Thành, HCM.
+- Ngày bắt đầu: 13/7/2015
+- Hình thức bảo hiểm: Xe trên 50cc có BH cho người trên xe
+3. Click "Tiếp theo" button.
+4. Click tab "2.Thông tin xe".
+5. Enter vehicle information:
+- Biển số đăng ký:60-Y6 6666
+- Nhãn hiệu: Honda
+- Số khung: 1001001
+- Số máy: 1001001
+- Dung tích: 110cc
+- Số loại: Air blade
+- Loại xe: Hai bánh
+- Màu sơn: Đỏ
+- Năm sản xuất: 2000
+- Tự trọng: 100
+- Số người: 2
+6. Click "TIẾP THEO" button.
+7. Click "TẠO HỢP ĐỒNG VÀ THANH TOÁN" button.</t>
   </si>
   <si>
-    <t>Show error message to notify that the contract not having a card.</t>
+    <t>Create contract successful, send an email contains customer code and password to customer. Request payment</t>
+  </si>
+  <si>
+    <t>RNC1,RNCP2.</t>
+  </si>
+  <si>
+    <t>1. Register new contract with information like test case "RNC1". And excute payment process like test case "RNCP2".
+2. Register another contract with information :
+- Họ tên: Nguyễn Văn B
+- Email: baohiem1@yahoo.com
+- Số điện thoại:0909888888
+- Số CMND/Hộ chiếu: 123485738
+- Địa chỉ: 123 Chợ Nhỏ, Bến Thành, HCM.
+- Ngày bắt đầu: 13/7/2015
+- Hình thức bảo hiểm: Xe trên 50cc có BH cho người trên xe
+- Biển số đăng ký:60-Y6 6666
+- Nhãn hiệu: Honda
+- Số khung: 1231231
+- Số máy: 1231231
+- Dung tích: 110cc
+- Số loại: Air blade
+- Loại xe: Hai bánh
+- Màu sơn: Đỏ
+- Năm sản xuất: 2000
+- Tự trọng: 100
+- Số người: 2</t>
+  </si>
+  <si>
+    <t>1. Register new contract with information like test case "RNC1".
+2. Go to the home page
+3. Enter personal information:
+- Họ tên: Nguyễn Văn B
+- Email: baohiem@yahoo.com
+- Số điện thoại:0909123123
+- Số CMND/Hộ chiếu: 123456789
+- Địa chỉ: 123 Chợ Bà Chiểu,Bình Thạnh, HCM.
+- Ngày bắt đầu: 13/7/2015
+- Hình thức bảo hiểm: Xe trên 50cc có BH cho người trên xe
+4. Click "Tiếp theo" button.</t>
+  </si>
+  <si>
+    <t>Show error message: "Email đã được đăng ký bởi người dùng khác"</t>
+  </si>
+  <si>
+    <t>Show error message:"Đang có hợp đồng hiệu lực với xe có biển số này"</t>
+  </si>
+  <si>
+    <t>1. Guest registered contract succeed like test case "RNC1".
+2. Guest choose direct payment.</t>
+  </si>
+  <si>
+    <t>1. Guest registered contract succeed like test case "RNC1".
+2. Guest choose PayPal payment.
+3. Guest log in and pay with PayPal web page.</t>
+  </si>
+  <si>
+    <t>Show success message:"Thanh toán thành công"</t>
+  </si>
+  <si>
+    <t>1. Guest registered contract succeed like test case "RNC1".
+2. Guest choose PayPal payment.
+3. Guest cancel transaction</t>
+  </si>
+  <si>
+    <t>Show message to notify that guest has canceled the transaction:"Bạn đã hủy thanh toán. Xin vui lòng Đăng nhập để thanh toán lại hoặc đến thanh toán trực tiếp"</t>
+  </si>
+  <si>
+    <t>Test send new card and deactivate old card request with direct payment.</t>
+  </si>
+  <si>
+    <t>Test send new card request with direct payment.</t>
+  </si>
+  <si>
+    <t>Test send new card and delivery request with PayPal payment</t>
+  </si>
+  <si>
+    <t>Test send new card request with PayPal payment.</t>
+  </si>
+  <si>
+    <t>Test send new card and deactivate old card request with PayPal payment.</t>
+  </si>
+  <si>
+    <t>Test send new card, deactivate old card and delivery request with PayPal payment</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán trực tiếp(tại công ty)"
+- Uncheck "Hủy bỏ thẻ cũ"
+3. Click "Xác nhận" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show success message:"Yêu cầu thẻ mới thành công. Vui lòng đến trực tiếp để thanh toán". Create new card request record and the old card been deactivated. </t>
+  </si>
+  <si>
+    <t>Show success message:"Yêu cầu thẻ mới thành công. Vui lòng đến trực tiếp để thanh toán". Create new card request record.</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán trực tiếp(tại công ty)"
+- Check "Hủy bỏ thẻ cũ"
+3. Click "Xác nhận" button.</t>
+  </si>
+  <si>
+    <t>SNCR6</t>
+  </si>
+  <si>
+    <t>SNCR7</t>
+  </si>
+  <si>
+    <t>SNCR8</t>
+  </si>
+  <si>
+    <t>Show success message:"Thanh toán thành công".Create new card request record.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show success message:"Thanh toán thành công".Create new card request record and the old card been deactivated. </t>
+  </si>
+  <si>
+    <t>Show success message:"Thanh toán thành công". Create new card request record with delivery requested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show success message:"Thanh toán thành công".Create new card request record with delivery requested and the old card been deactivated. </t>
+  </si>
+  <si>
+    <t>SNCR9</t>
+  </si>
+  <si>
+    <t>Test send new card request with PayPal payment but user cancel payment process</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán qua PayPal"
+- Uncheck "Hủy bỏ thẻ cũ"
+- Check "Nhận thẻ tại công ty"
+3. Click "Xác nhận" button.
+4. User log in and pay with PayPal web page.</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán qua PayPal"
+- Check "Hủy bỏ thẻ cũ"
+- Check "Nhận thẻ tại công ty"
+3. Click "Xác nhận" button.
+4. User log in and pay with PayPal web page.</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán qua PayPal"
+- Uncheck "Hủy bỏ thẻ cũ"
+- Uncheck "Nhận thẻ tại công ty"
+3. Click "Xác nhận" button.
+4. User log in and pay with PayPal web page.</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán qua PayPal"
+- Check "Hủy bỏ thẻ cũ"
+- Uncheck "Nhận thẻ tại công ty"
+3. Click "Xác nhận" button.
+4. User log in and pay with PayPal web page.</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card. No new card request before.
+2. In "Yêu Cầu Thẻ Mới" page for contract HD0001, input fields:
+- Mật khẩu: correct password
+- Ghi chú: "Làm lại thẻ".
+- Choose: "Thanh toán qua PayPal"
+- Uncheck "Hủy bỏ thẻ cũ"
+- Check "Nhận thẻ tại công ty"
+3. Click "Xác nhận" button.
+4. User cancel PayPal payment process.</t>
+  </si>
+  <si>
+    <t>Show error message:"Bạn đã hủy thanh toán. Xin vui lòng thực hiện lại hoặc đến thanh toán trực tiếp"</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 having an actived card with a new card request before.
+2. Send new card request for contract HD0001 like test case SNCR1.</t>
+  </si>
+  <si>
+    <t>Show error message:"Bạn đã yêu cầu thẻ mới trước đó. Vui lòng chờ xử lý"</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 not having a card.
+2. Send new card request for contract HD0001 like test case SNCR1.</t>
+  </si>
+  <si>
+    <t>Show error message:"Hợp đồng chưa có thẻ bảo hiểm. Xin vui lòng đợi phát hành"</t>
+  </si>
+  <si>
+    <t>1. Create 5 new card request with 5 different request date.
+2. Click "Yêu cầu thẻ mới" bar.</t>
+  </si>
+  <si>
+    <t>1. Crete 5 new card request with the same request date. But 2 of them is resolved.
+2. Click "Yêu cầu thẻ mới" bar.</t>
+  </si>
+  <si>
+    <t>Display the list new card requests in ascending order of request date.</t>
+  </si>
+  <si>
+    <t>Display 3 unresolved new card requests on top and 2 resolved new card request on bottom.</t>
   </si>
 </sst>
 </file>
@@ -616,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -710,13 +860,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
+      <c r="C3" s="7" t="s">
+        <v>38</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
@@ -749,16 +899,18 @@
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
+      <c r="C4" s="7" t="s">
+        <v>41</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
+      <c r="D4" s="7" t="s">
+        <v>44</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
@@ -789,16 +941,18 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>34</v>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
+      <c r="C5" s="7" t="s">
+        <v>42</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
+      <c r="D5" s="7" t="s">
+        <v>43</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
@@ -827,7 +981,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -901,18 +1055,20 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
@@ -940,19 +1096,21 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
+      <c r="A9" s="7" t="s">
+        <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>36</v>
+      <c r="B9" s="7" t="s">
+        <v>25</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
+      <c r="C9" s="7" t="s">
+        <v>46</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="4" t="s">
         <v>8</v>
       </c>
@@ -981,18 +1139,20 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>37</v>
+      <c r="B10" s="7" t="s">
+        <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1021,7 +1181,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1095,18 +1255,20 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>39</v>
+      <c r="D13" s="7" t="s">
+        <v>81</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="F13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1135,18 +1297,20 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1339,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1305,7 +1469,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1379,16 +1543,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="7" t="s">
@@ -1419,16 +1583,16 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="7" t="s">
@@ -1459,24 +1623,20 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="3">
-        <v>42198</v>
-      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1499,24 +1659,20 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="3">
-        <v>42198</v>
-      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1537,15 +1693,15 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>65</v>
@@ -1577,14 +1733,22 @@
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1605,14 +1769,22 @@
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1633,14 +1805,28 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="3">
+        <v>42198</v>
+      </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1661,14 +1847,28 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+    <row r="29" spans="1:26" ht="66" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="3">
+        <v>42198</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -28737,6 +28937,118 @@
       <c r="Y995" s="4"/>
       <c r="Z995" s="4"/>
     </row>
+    <row r="996" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A996" s="4"/>
+      <c r="B996" s="4"/>
+      <c r="C996" s="4"/>
+      <c r="D996" s="4"/>
+      <c r="E996" s="4"/>
+      <c r="F996" s="4"/>
+      <c r="G996" s="4"/>
+      <c r="H996" s="4"/>
+      <c r="I996" s="4"/>
+      <c r="J996" s="4"/>
+      <c r="K996" s="4"/>
+      <c r="L996" s="4"/>
+      <c r="M996" s="4"/>
+      <c r="N996" s="4"/>
+      <c r="O996" s="4"/>
+      <c r="P996" s="4"/>
+      <c r="Q996" s="4"/>
+      <c r="R996" s="4"/>
+      <c r="S996" s="4"/>
+      <c r="T996" s="4"/>
+      <c r="U996" s="4"/>
+      <c r="V996" s="4"/>
+      <c r="W996" s="4"/>
+      <c r="X996" s="4"/>
+      <c r="Y996" s="4"/>
+      <c r="Z996" s="4"/>
+    </row>
+    <row r="997" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A997" s="4"/>
+      <c r="B997" s="4"/>
+      <c r="C997" s="4"/>
+      <c r="D997" s="4"/>
+      <c r="E997" s="4"/>
+      <c r="F997" s="4"/>
+      <c r="G997" s="4"/>
+      <c r="H997" s="4"/>
+      <c r="I997" s="4"/>
+      <c r="J997" s="4"/>
+      <c r="K997" s="4"/>
+      <c r="L997" s="4"/>
+      <c r="M997" s="4"/>
+      <c r="N997" s="4"/>
+      <c r="O997" s="4"/>
+      <c r="P997" s="4"/>
+      <c r="Q997" s="4"/>
+      <c r="R997" s="4"/>
+      <c r="S997" s="4"/>
+      <c r="T997" s="4"/>
+      <c r="U997" s="4"/>
+      <c r="V997" s="4"/>
+      <c r="W997" s="4"/>
+      <c r="X997" s="4"/>
+      <c r="Y997" s="4"/>
+      <c r="Z997" s="4"/>
+    </row>
+    <row r="998" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A998" s="4"/>
+      <c r="B998" s="4"/>
+      <c r="C998" s="4"/>
+      <c r="D998" s="4"/>
+      <c r="E998" s="4"/>
+      <c r="F998" s="4"/>
+      <c r="G998" s="4"/>
+      <c r="H998" s="4"/>
+      <c r="I998" s="4"/>
+      <c r="J998" s="4"/>
+      <c r="K998" s="4"/>
+      <c r="L998" s="4"/>
+      <c r="M998" s="4"/>
+      <c r="N998" s="4"/>
+      <c r="O998" s="4"/>
+      <c r="P998" s="4"/>
+      <c r="Q998" s="4"/>
+      <c r="R998" s="4"/>
+      <c r="S998" s="4"/>
+      <c r="T998" s="4"/>
+      <c r="U998" s="4"/>
+      <c r="V998" s="4"/>
+      <c r="W998" s="4"/>
+      <c r="X998" s="4"/>
+      <c r="Y998" s="4"/>
+      <c r="Z998" s="4"/>
+    </row>
+    <row r="999" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A999" s="4"/>
+      <c r="B999" s="4"/>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
+      <c r="H999" s="4"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+      <c r="K999" s="4"/>
+      <c r="L999" s="4"/>
+      <c r="M999" s="4"/>
+      <c r="N999" s="4"/>
+      <c r="O999" s="4"/>
+      <c r="P999" s="4"/>
+      <c r="Q999" s="4"/>
+      <c r="R999" s="4"/>
+      <c r="S999" s="4"/>
+      <c r="T999" s="4"/>
+      <c r="U999" s="4"/>
+      <c r="V999" s="4"/>
+      <c r="W999" s="4"/>
+      <c r="X999" s="4"/>
+      <c r="Y999" s="4"/>
+      <c r="Z999" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add test case for resolve new card request #308
</commit_message>
<xml_diff>
--- a/Document/Reports/Report 5/Test case- TriPQM.xlsx
+++ b/Document/Reports/Report 5/Test case- TriPQM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -377,6 +377,23 @@
   </si>
   <si>
     <t>Display 3 unresolved new card requests on top and 2 resolved new card request on bottom.</t>
+  </si>
+  <si>
+    <t>RNCR1</t>
+  </si>
+  <si>
+    <t>Test resolve new card request, print a new card</t>
+  </si>
+  <si>
+    <t>1. Contract HD0001 is Ready and having an actived card.
+2. Create new card request for contract HD001 like test case SNCR1.
+3. Print card for Ready contract "HD0001" like test case PC2.</t>
+  </si>
+  <si>
+    <t>SNCR1,PC2.</t>
+  </si>
+  <si>
+    <t>Printer app show message "Write success", contract card change to new card ID, old card is deactivated</t>
   </si>
 </sst>
 </file>
@@ -766,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1412,13 +1429,27 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>42198</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1440,7 +1471,9 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1468,16 +1501,30 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>30</v>
+      <c r="A19" s="2" t="s">
+        <v>0</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1498,30 +1545,26 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>0</v>
+      <c r="A20" s="7" t="s">
+        <v>31</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>2</v>
+      <c r="C20" s="7" t="s">
+        <v>56</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>3</v>
+      <c r="D20" s="7" t="s">
+        <v>58</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>4</v>
+      <c r="E20" s="4"/>
+      <c r="F20" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>5</v>
+      <c r="G20" s="3">
+        <v>42198</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1543,16 +1586,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="7" t="s">
@@ -1583,16 +1626,16 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="7" t="s">
@@ -1623,20 +1666,24 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="3"/>
+      <c r="F23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="3">
+        <v>42198</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1659,20 +1706,24 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="3"/>
+      <c r="F24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="3">
+        <v>42198</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1695,16 +1746,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="7" t="s">
@@ -1735,20 +1786,24 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>42198</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1771,20 +1826,26 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="3"/>
+      <c r="E27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="3">
+        <v>42198</v>
+      </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1805,18 +1866,18 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>31</v>
@@ -1847,28 +1908,14 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row r="29" spans="1:26" ht="66" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="3">
-        <v>42198</v>
-      </c>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -29021,34 +29068,6 @@
       <c r="Y998" s="4"/>
       <c r="Z998" s="4"/>
     </row>
-    <row r="999" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A999" s="4"/>
-      <c r="B999" s="4"/>
-      <c r="C999" s="4"/>
-      <c r="D999" s="4"/>
-      <c r="E999" s="4"/>
-      <c r="F999" s="4"/>
-      <c r="G999" s="4"/>
-      <c r="H999" s="4"/>
-      <c r="I999" s="4"/>
-      <c r="J999" s="4"/>
-      <c r="K999" s="4"/>
-      <c r="L999" s="4"/>
-      <c r="M999" s="4"/>
-      <c r="N999" s="4"/>
-      <c r="O999" s="4"/>
-      <c r="P999" s="4"/>
-      <c r="Q999" s="4"/>
-      <c r="R999" s="4"/>
-      <c r="S999" s="4"/>
-      <c r="T999" s="4"/>
-      <c r="U999" s="4"/>
-      <c r="V999" s="4"/>
-      <c r="W999" s="4"/>
-      <c r="X999" s="4"/>
-      <c r="Y999" s="4"/>
-      <c r="Z999" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>